<commit_message>
Removed Result columns from excel sheets and updated data providers
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/hybridFrameworkTestDriver.xlsx
+++ b/src/test/resources/testdata/hybridFrameworkTestDriver.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saura\eclipse-workspace\HybridFrameworkProjectTemplate\src\test\resources\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saura\eclipse-workspace\HybridMultiThreadedProjectTemplate\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D670B551-72CD-4037-9CA8-05D33E6C6632}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{470938A7-ED58-40CB-BBAB-6196FB8C8929}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Driver" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="81">
   <si>
     <t>Choose Test (Smoke/Regression/Custom/Negative)</t>
   </si>
@@ -57,12 +57,6 @@
   </si>
   <si>
     <t>Groups</t>
-  </si>
-  <si>
-    <t>PassPercentage</t>
-  </si>
-  <si>
-    <t>Result</t>
   </si>
   <si>
     <t xml:space="preserve">Y </t>
@@ -329,12 +323,6 @@
     <t>TC_0006_1</t>
   </si>
   <si>
-    <t>PASS</t>
-  </si>
-  <si>
-    <t>100.0 %</t>
-  </si>
-  <si>
     <t>ExpHomePageHeader</t>
   </si>
   <si>
@@ -397,9 +385,6 @@
     <t>TC_0006_2</t>
   </si>
   <si>
-    <t>FAIL</t>
-  </si>
-  <si>
     <t>https://nirajt03.github.io/sample-website/</t>
   </si>
   <si>
@@ -410,15 +395,6 @@
   </si>
   <si>
     <t>pragyan@123</t>
-  </si>
-  <si>
-    <t>33.33 %</t>
-  </si>
-  <si>
-    <t>0.0 %</t>
-  </si>
-  <si>
-    <t>66.67 %</t>
   </si>
 </sst>
 </file>
@@ -530,7 +506,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -578,21 +554,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="50"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="13">
     <border>
@@ -760,7 +721,7 @@
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0"/>
     <xf numFmtId="43" fontId="9" fillId="7" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="406">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -775,7 +736,6 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -805,7 +765,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -846,371 +805,9 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Comma 2" xfId="10" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1509,16 +1106,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="43.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.19921875" collapsed="true"/>
+    <col min="1" max="1" width="43" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.19921875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22" t="s">
-        <v>75</v>
+      <c r="B1" s="21" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1542,8 +1139,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="8.19921875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="37.0" collapsed="true"/>
+    <col min="1" max="1" width="8.19921875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="37" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.45">
@@ -1555,11 +1152,11 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="42" t="s">
-        <v>82</v>
+      <c r="B2" s="39" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
@@ -1585,23 +1182,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="8.1328125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="49.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="33.59765625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.19921875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="15.6640625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="6.6640625" collapsed="true"/>
+    <col min="1" max="1" width="8.1328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="49" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="33.59765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.19921875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="6" t="s">
         <v>4</v>
       </c>
@@ -1614,131 +1209,89 @@
       <c r="D1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="9" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A2" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="B2" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="18" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A2" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="F2" t="s" s="387">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A3" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="17" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A3" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A4" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A5" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C5" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="D3" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="F3" t="s" s="393">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A4" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="17" t="s">
+      <c r="D5" s="24" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A6" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C6" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D6" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="F4" t="s" s="399">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A5" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="17" t="s">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A7" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C7" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D7" s="24" t="s">
         <v>52</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="F5" t="s" s="396">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A6" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="D6" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="F6" t="s" s="402">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A7" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="D7" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="F7" t="s" s="405">
-        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1762,90 +1315,80 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="9.53125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.265625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.59765625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.06640625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="12.796875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="24.46484375" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="7.6640625" collapsed="true"/>
+    <col min="1" max="1" width="9.53125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.59765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.06640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="24.46484375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A1" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="43" t="s">
+      <c r="B3" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A2" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="44" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="E2" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="F2" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="G2" s="385" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A3" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="C3" s="44" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="F3" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3" s="386" t="s">
-        <v>59</v>
+      <c r="D3" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1862,132 +1405,113 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50E7E38D-2134-4D7B-AFCC-79142EC6D7FA}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="9.53125"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.265625"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.06640625"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.265625"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="27.33203125"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="6.6640625"/>
+    <col min="1" max="1" width="9.53125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.06640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A1" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A2" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A3" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A2" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="13" t="s">
+      <c r="B3" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A4" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C4" s="13"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A5" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A6" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="13"/>
+      <c r="D6" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="F2" s="388" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A3" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="15" t="s">
+      <c r="E6" s="14" t="s">
         <v>37</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="F3" s="389" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A4" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="F4" s="390" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A5" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="F5" s="391" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A6" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" s="14"/>
-      <c r="D6" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="E6" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="F6" s="392" t="s">
-        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -2003,109 +1527,99 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B881C555-7FA8-4DD1-A7D0-F5D26883CF57}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B3"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="9.53125"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.265625"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.59765625"/>
-    <col min="4" max="5" bestFit="true" customWidth="true" width="36.06640625"/>
-    <col min="6" max="6" customWidth="true" width="69.46484375"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="22.33203125"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="23.59765625"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="6.6640625"/>
+    <col min="1" max="1" width="9.53125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="36.06640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="69.46484375" customWidth="1"/>
+    <col min="7" max="7" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A1" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="32" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="54" x14ac:dyDescent="0.45">
+      <c r="A2" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" s="36" t="s">
+        <v>62</v>
+      </c>
+      <c r="F2" s="37" t="s">
+        <v>67</v>
+      </c>
+      <c r="G2" s="36" t="s">
+        <v>68</v>
+      </c>
+      <c r="H2" s="37" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="54" x14ac:dyDescent="0.45">
+      <c r="A3" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="20" t="s">
+      <c r="B3" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="34" t="s">
-        <v>65</v>
-      </c>
-      <c r="E1" s="9" t="s">
+      <c r="D3" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" s="36" t="s">
+        <v>62</v>
+      </c>
+      <c r="F3" s="37" t="s">
+        <v>67</v>
+      </c>
+      <c r="G3" s="36" t="s">
+        <v>68</v>
+      </c>
+      <c r="H3" s="36" t="s">
         <v>69</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="54" x14ac:dyDescent="0.45">
-      <c r="A2" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="31" t="s">
-        <v>55</v>
-      </c>
-      <c r="C2" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="40" t="s">
-        <v>66</v>
-      </c>
-      <c r="E2" s="38" t="s">
-        <v>66</v>
-      </c>
-      <c r="F2" s="39" t="s">
-        <v>71</v>
-      </c>
-      <c r="G2" s="38" t="s">
-        <v>72</v>
-      </c>
-      <c r="H2" s="39" t="s">
-        <v>73</v>
-      </c>
-      <c r="I2" s="394" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="54" x14ac:dyDescent="0.45">
-      <c r="A3" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="31" t="s">
-        <v>79</v>
-      </c>
-      <c r="C3" s="37" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="40" t="s">
-        <v>66</v>
-      </c>
-      <c r="E3" s="38" t="s">
-        <v>66</v>
-      </c>
-      <c r="F3" s="39" t="s">
-        <v>71</v>
-      </c>
-      <c r="G3" s="38" t="s">
-        <v>72</v>
-      </c>
-      <c r="H3" s="38" t="s">
-        <v>73</v>
-      </c>
-      <c r="I3" s="395" t="s">
-        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -2121,80 +1635,70 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3356B94C-5B4C-4FFF-9F00-EBBCCEB4F868}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B3"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="9.53125"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.265625"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.59765625"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="22.06640625"/>
-    <col min="5" max="5" customWidth="true" width="59.59765625"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="6.6640625"/>
+    <col min="1" max="1" width="9.53125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.06640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="59.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A1" s="27" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A1" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="28" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="54" x14ac:dyDescent="0.45">
+      <c r="A2" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="31" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="54" x14ac:dyDescent="0.45">
+      <c r="A3" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="28" t="s">
+      <c r="B3" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="E1" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="F1" s="30" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="54" x14ac:dyDescent="0.45">
-      <c r="A2" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="31" t="s">
-        <v>56</v>
-      </c>
-      <c r="C2" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="33" t="s">
-        <v>63</v>
-      </c>
-      <c r="E2" s="33" t="s">
-        <v>64</v>
-      </c>
-      <c r="F2" s="397" t="s">
+      <c r="D3" s="31" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="54" x14ac:dyDescent="0.45">
-      <c r="A3" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="31" t="s">
-        <v>78</v>
-      </c>
-      <c r="C3" s="32" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="33" t="s">
-        <v>63</v>
-      </c>
-      <c r="E3" s="33" t="s">
-        <v>64</v>
-      </c>
-      <c r="F3" s="398" t="s">
-        <v>59</v>
+      <c r="E3" s="31" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -2211,69 +1715,60 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B8C79C5-CBC0-4DDF-9AC8-C72E09C8FEF2}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B3"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="9.53125"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.265625"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.59765625"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.6640625"/>
+    <col min="1" max="1" width="9.53125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A1" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A2" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A3" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="20" t="s">
+      <c r="B3" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A2" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="C2" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="E2" s="400" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A3" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="C3" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="E3" s="401" t="s">
-        <v>59</v>
+      <c r="D3" s="14" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -2289,89 +1784,79 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53B62C1C-0C0C-47DD-9D4A-D15FCE655D45}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="9.53125"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.265625"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.59765625"/>
-    <col min="4" max="5" bestFit="true" customWidth="true" width="36.06640625"/>
-    <col min="6" max="6" customWidth="true" style="36" width="69.53125"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="6.6640625"/>
+    <col min="1" max="1" width="9.53125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="36.06640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="69.53125" style="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A1" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" s="33" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="40.5" x14ac:dyDescent="0.45">
+      <c r="A2" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="36" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" s="36" t="s">
+        <v>62</v>
+      </c>
+      <c r="F2" s="37" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="40.5" x14ac:dyDescent="0.45">
+      <c r="A3" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="20" t="s">
+      <c r="B3" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="F1" s="35" t="s">
-        <v>70</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="40.5" x14ac:dyDescent="0.45">
-      <c r="A2" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="C2" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="38" t="s">
-        <v>66</v>
-      </c>
-      <c r="E2" s="38" t="s">
-        <v>66</v>
-      </c>
-      <c r="F2" s="39" t="s">
-        <v>71</v>
-      </c>
-      <c r="G2" s="403" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="40.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="C3" s="37" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="38" t="s">
-        <v>66</v>
-      </c>
-      <c r="E3" s="38" t="s">
-        <v>66</v>
-      </c>
-      <c r="F3" s="39" t="s">
-        <v>71</v>
-      </c>
-      <c r="G3" s="404" t="s">
-        <v>59</v>
+      <c r="D3" s="36" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" s="36" t="s">
+        <v>62</v>
+      </c>
+      <c r="F3" s="37" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>